<commit_message>
update latest data to 2023
</commit_message>
<xml_diff>
--- a/Data_raw.xlsx
+++ b/Data_raw.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView windowWidth="24045" windowHeight="12255" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Capacity_solar" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="Cost_wind" sheetId="4" r:id="rId4"/>
     <sheet name="Scn_nat_solar" sheetId="5" r:id="rId5"/>
     <sheet name="Scn_nat_wind" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
@@ -100,7 +124,13 @@
     <t>price_si</t>
   </si>
   <si>
+    <t>2023N</t>
+  </si>
+  <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t>const</t>
@@ -1036,11 +1066,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2304,11 +2334,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="A1" sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3947,14 +3977,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:O14"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="O2" sqref="O2:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="3" max="3" width="12.625"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
@@ -4609,6 +4642,105 @@
       </c>
       <c r="O14">
         <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>731</v>
+      </c>
+      <c r="C15">
+        <f>ROUND($B15/$B16*C16,0)</f>
+        <v>954</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:M15" si="0">ROUND($B15/$B16*D16,0)</f>
+        <v>921</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>686</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>792</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1808</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>1162</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>647</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1069</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>647</v>
+      </c>
+      <c r="N15">
+        <v>795.67</v>
+      </c>
+      <c r="O15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>758</v>
+      </c>
+      <c r="C16">
+        <v>989</v>
+      </c>
+      <c r="D16">
+        <v>955</v>
+      </c>
+      <c r="E16">
+        <v>731</v>
+      </c>
+      <c r="F16">
+        <v>711</v>
+      </c>
+      <c r="G16">
+        <v>821</v>
+      </c>
+      <c r="H16">
+        <v>1875</v>
+      </c>
+      <c r="I16">
+        <v>1205</v>
+      </c>
+      <c r="J16">
+        <v>671</v>
+      </c>
+      <c r="K16">
+        <v>933</v>
+      </c>
+      <c r="L16">
+        <v>1109</v>
+      </c>
+      <c r="M16">
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -4620,18 +4752,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:P14"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="12.625"/>
+    <col min="4" max="4" width="12.625"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -5327,6 +5463,117 @@
       </c>
       <c r="P14">
         <v>1596.07574731528</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <f>ROUND(B14/1322*B16,3)</f>
+        <v>1118.044</v>
+      </c>
+      <c r="C15">
+        <f>C14</f>
+        <v>2131.67</v>
+      </c>
+      <c r="D15">
+        <f>ROUND($B15/$B16*D16,2)</f>
+        <v>1446.71</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:O15" si="0">ROUND($B15/$B16*E16,2)</f>
+        <v>1686.7</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1479.48</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1319.48</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1226.96</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>1164.31</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>1116.12</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>1368.64</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1682.85</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>1382.13</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>1039.97</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>950.34</v>
+      </c>
+      <c r="P15">
+        <v>1499.08396690286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>1160</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>1501</v>
+      </c>
+      <c r="E16">
+        <v>1750</v>
+      </c>
+      <c r="F16">
+        <v>1535</v>
+      </c>
+      <c r="G16">
+        <v>1369</v>
+      </c>
+      <c r="H16">
+        <v>1273</v>
+      </c>
+      <c r="I16">
+        <v>1208</v>
+      </c>
+      <c r="J16">
+        <v>1158</v>
+      </c>
+      <c r="K16">
+        <v>1420</v>
+      </c>
+      <c r="L16">
+        <v>1746</v>
+      </c>
+      <c r="M16">
+        <v>1434</v>
+      </c>
+      <c r="N16">
+        <v>1079</v>
+      </c>
+      <c r="O16">
+        <v>986</v>
       </c>
     </row>
   </sheetData>
@@ -5337,7 +5584,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5393,7 +5640,7 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -6604,7 +6851,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6666,7 +6913,7 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -8011,6 +8258,2885 @@
       </c>
       <c r="R25">
         <v>181.08267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:N34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="4" width="11.5"/>
+    <col min="5" max="5" width="10.375"/>
+    <col min="6" max="7" width="12.625"/>
+    <col min="8" max="8" width="10.375"/>
+    <col min="9" max="10" width="11.5"/>
+    <col min="11" max="12" width="12.625"/>
+    <col min="13" max="13" width="11.5"/>
+    <col min="14" max="15" width="12.625"/>
+    <col min="17" max="17" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>5124</v>
+      </c>
+      <c r="C2">
+        <v>7749</v>
+      </c>
+      <c r="D2">
+        <v>6137</v>
+      </c>
+      <c r="E2">
+        <v>4157</v>
+      </c>
+      <c r="F2">
+        <v>5667</v>
+      </c>
+      <c r="G2">
+        <v>5811</v>
+      </c>
+      <c r="I2">
+        <v>10089</v>
+      </c>
+      <c r="J2">
+        <v>5241</v>
+      </c>
+      <c r="K2">
+        <v>6634</v>
+      </c>
+      <c r="L2">
+        <v>5142</v>
+      </c>
+      <c r="M2">
+        <v>4104</v>
+      </c>
+      <c r="N2">
+        <v>7978.91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>4329</v>
+      </c>
+      <c r="C3">
+        <v>7603</v>
+      </c>
+      <c r="D3">
+        <v>6274</v>
+      </c>
+      <c r="E3">
+        <v>3306</v>
+      </c>
+      <c r="F3">
+        <v>3491</v>
+      </c>
+      <c r="G3">
+        <v>5446</v>
+      </c>
+      <c r="H3">
+        <v>6093</v>
+      </c>
+      <c r="I3">
+        <v>6621</v>
+      </c>
+      <c r="J3">
+        <v>3661</v>
+      </c>
+      <c r="K3">
+        <v>5273</v>
+      </c>
+      <c r="L3">
+        <v>5039</v>
+      </c>
+      <c r="M3">
+        <v>3816</v>
+      </c>
+      <c r="N3">
+        <v>5346.425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>3343</v>
+      </c>
+      <c r="C4">
+        <v>5507</v>
+      </c>
+      <c r="D4">
+        <v>5549</v>
+      </c>
+      <c r="E4">
+        <v>2627</v>
+      </c>
+      <c r="F4">
+        <v>3063</v>
+      </c>
+      <c r="G4">
+        <v>2884</v>
+      </c>
+      <c r="H4">
+        <v>4396</v>
+      </c>
+      <c r="I4">
+        <v>2570</v>
+      </c>
+      <c r="J4">
+        <v>3016</v>
+      </c>
+      <c r="K4">
+        <v>3120</v>
+      </c>
+      <c r="L4">
+        <v>4955</v>
+      </c>
+      <c r="M4">
+        <v>3076</v>
+      </c>
+      <c r="N4">
+        <v>2713.94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>2935</v>
+      </c>
+      <c r="C5">
+        <v>3232</v>
+      </c>
+      <c r="D5">
+        <v>3641</v>
+      </c>
+      <c r="E5">
+        <v>2252</v>
+      </c>
+      <c r="F5">
+        <v>3153</v>
+      </c>
+      <c r="G5">
+        <v>2284</v>
+      </c>
+      <c r="H5">
+        <v>3756</v>
+      </c>
+      <c r="I5">
+        <v>2987</v>
+      </c>
+      <c r="J5">
+        <v>2591</v>
+      </c>
+      <c r="K5">
+        <v>2587</v>
+      </c>
+      <c r="L5">
+        <v>4392</v>
+      </c>
+      <c r="M5">
+        <v>2375</v>
+      </c>
+      <c r="N5">
+        <v>2489.77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>2652</v>
+      </c>
+      <c r="C6">
+        <v>3374</v>
+      </c>
+      <c r="D6">
+        <v>2658</v>
+      </c>
+      <c r="E6">
+        <v>1795</v>
+      </c>
+      <c r="F6">
+        <v>2140</v>
+      </c>
+      <c r="G6">
+        <v>2212</v>
+      </c>
+      <c r="H6">
+        <v>3443</v>
+      </c>
+      <c r="I6">
+        <v>2481</v>
+      </c>
+      <c r="J6">
+        <v>2598</v>
+      </c>
+      <c r="K6">
+        <v>2180</v>
+      </c>
+      <c r="L6">
+        <v>3237</v>
+      </c>
+      <c r="M6">
+        <v>1978</v>
+      </c>
+      <c r="N6">
+        <v>2509.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>2016</v>
+      </c>
+      <c r="C7">
+        <v>2509</v>
+      </c>
+      <c r="D7">
+        <v>1749</v>
+      </c>
+      <c r="E7">
+        <v>1436</v>
+      </c>
+      <c r="F7">
+        <v>1458</v>
+      </c>
+      <c r="G7">
+        <v>1838.33</v>
+      </c>
+      <c r="H7">
+        <v>2491</v>
+      </c>
+      <c r="I7">
+        <v>2346</v>
+      </c>
+      <c r="J7">
+        <v>1340</v>
+      </c>
+      <c r="K7">
+        <v>1715</v>
+      </c>
+      <c r="L7">
+        <v>2885</v>
+      </c>
+      <c r="M7">
+        <v>1528</v>
+      </c>
+      <c r="N7">
+        <v>1954.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>1833</v>
+      </c>
+      <c r="C8">
+        <v>2160</v>
+      </c>
+      <c r="D8">
+        <v>1481</v>
+      </c>
+      <c r="E8">
+        <v>1303</v>
+      </c>
+      <c r="F8">
+        <v>1255</v>
+      </c>
+      <c r="G8">
+        <v>1464.66</v>
+      </c>
+      <c r="H8">
+        <v>2734</v>
+      </c>
+      <c r="I8">
+        <v>2315</v>
+      </c>
+      <c r="J8">
+        <v>1220</v>
+      </c>
+      <c r="K8">
+        <v>1643</v>
+      </c>
+      <c r="L8">
+        <v>2492</v>
+      </c>
+      <c r="M8">
+        <v>1384</v>
+      </c>
+      <c r="N8">
+        <v>2354.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>1586</v>
+      </c>
+      <c r="C9">
+        <v>2211</v>
+      </c>
+      <c r="D9">
+        <v>1391</v>
+      </c>
+      <c r="E9">
+        <v>1250</v>
+      </c>
+      <c r="F9">
+        <v>1252</v>
+      </c>
+      <c r="G9">
+        <v>1091</v>
+      </c>
+      <c r="H9">
+        <v>2480</v>
+      </c>
+      <c r="I9">
+        <v>1774</v>
+      </c>
+      <c r="J9">
+        <v>1100</v>
+      </c>
+      <c r="K9">
+        <v>1421</v>
+      </c>
+      <c r="L9">
+        <v>2101</v>
+      </c>
+      <c r="M9">
+        <v>1298</v>
+      </c>
+      <c r="N9">
+        <v>2207.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>1355</v>
+      </c>
+      <c r="C10">
+        <v>1705</v>
+      </c>
+      <c r="D10">
+        <v>1205</v>
+      </c>
+      <c r="E10">
+        <v>1249</v>
+      </c>
+      <c r="F10">
+        <v>889</v>
+      </c>
+      <c r="G10">
+        <v>976</v>
+      </c>
+      <c r="H10">
+        <v>2357</v>
+      </c>
+      <c r="I10">
+        <v>1488</v>
+      </c>
+      <c r="J10">
+        <v>980</v>
+      </c>
+      <c r="K10">
+        <v>1528</v>
+      </c>
+      <c r="L10">
+        <v>1737</v>
+      </c>
+      <c r="M10">
+        <v>987</v>
+      </c>
+      <c r="N10">
+        <v>1996.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>1120</v>
+      </c>
+      <c r="C11">
+        <v>1403</v>
+      </c>
+      <c r="D11">
+        <v>1098</v>
+      </c>
+      <c r="E11">
+        <v>1008</v>
+      </c>
+      <c r="F11">
+        <v>694</v>
+      </c>
+      <c r="G11">
+        <v>931</v>
+      </c>
+      <c r="H11">
+        <v>2322</v>
+      </c>
+      <c r="I11">
+        <v>1405</v>
+      </c>
+      <c r="J11">
+        <v>860</v>
+      </c>
+      <c r="K11">
+        <v>1142</v>
+      </c>
+      <c r="L11">
+        <v>1369</v>
+      </c>
+      <c r="M11">
+        <v>891</v>
+      </c>
+      <c r="N11">
+        <v>1073.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>983</v>
+      </c>
+      <c r="C12">
+        <v>1176</v>
+      </c>
+      <c r="D12">
+        <v>1045</v>
+      </c>
+      <c r="E12">
+        <v>776</v>
+      </c>
+      <c r="F12">
+        <v>661</v>
+      </c>
+      <c r="G12">
+        <v>866</v>
+      </c>
+      <c r="H12">
+        <v>2031</v>
+      </c>
+      <c r="I12">
+        <v>1052</v>
+      </c>
+      <c r="J12">
+        <v>845</v>
+      </c>
+      <c r="K12">
+        <v>937</v>
+      </c>
+      <c r="L12">
+        <v>1241</v>
+      </c>
+      <c r="M12">
+        <v>721</v>
+      </c>
+      <c r="N12">
+        <v>1076.31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>917</v>
+      </c>
+      <c r="C13">
+        <v>1095</v>
+      </c>
+      <c r="D13">
+        <v>865</v>
+      </c>
+      <c r="E13">
+        <v>742</v>
+      </c>
+      <c r="F13">
+        <v>631</v>
+      </c>
+      <c r="G13">
+        <v>840</v>
+      </c>
+      <c r="H13">
+        <v>1812</v>
+      </c>
+      <c r="I13">
+        <v>1006</v>
+      </c>
+      <c r="J13">
+        <v>873</v>
+      </c>
+      <c r="K13">
+        <v>907</v>
+      </c>
+      <c r="L13">
+        <v>1162</v>
+      </c>
+      <c r="M13">
+        <v>672</v>
+      </c>
+      <c r="N13">
+        <v>1147.23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>876</v>
+      </c>
+      <c r="C14">
+        <v>923</v>
+      </c>
+      <c r="D14">
+        <v>1157</v>
+      </c>
+      <c r="E14">
+        <v>996</v>
+      </c>
+      <c r="F14">
+        <v>640</v>
+      </c>
+      <c r="G14">
+        <v>771</v>
+      </c>
+      <c r="H14">
+        <v>1905</v>
+      </c>
+      <c r="I14">
+        <v>1338</v>
+      </c>
+      <c r="J14">
+        <v>778</v>
+      </c>
+      <c r="K14">
+        <v>910</v>
+      </c>
+      <c r="L14">
+        <v>1119</v>
+      </c>
+      <c r="M14">
+        <v>715</v>
+      </c>
+      <c r="N14">
+        <v>998.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>731</v>
+      </c>
+      <c r="C15">
+        <v>954</v>
+      </c>
+      <c r="D15">
+        <v>921</v>
+      </c>
+      <c r="E15">
+        <v>705</v>
+      </c>
+      <c r="F15">
+        <v>686</v>
+      </c>
+      <c r="G15">
+        <v>792</v>
+      </c>
+      <c r="H15">
+        <v>1808</v>
+      </c>
+      <c r="I15">
+        <v>1162</v>
+      </c>
+      <c r="J15">
+        <v>647</v>
+      </c>
+      <c r="K15">
+        <v>900</v>
+      </c>
+      <c r="L15">
+        <v>1069</v>
+      </c>
+      <c r="M15">
+        <v>647</v>
+      </c>
+      <c r="N15" cm="1">
+        <f t="array" ref="N15">ROUND((B15*B34-SUM(C15:M15*C34:M34))/N34,2)</f>
+        <v>795.67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21">
+        <v>2010</v>
+      </c>
+      <c r="B21">
+        <v>17.990818</v>
+      </c>
+      <c r="C21">
+        <v>0.75900008</v>
+      </c>
+      <c r="D21">
+        <v>0.767</v>
+      </c>
+      <c r="E21">
+        <v>7.439999</v>
+      </c>
+      <c r="F21">
+        <v>0.025999998</v>
+      </c>
+      <c r="G21">
+        <v>2.3327202</v>
+      </c>
+      <c r="H21">
+        <v>0.9910003</v>
+      </c>
+      <c r="I21">
+        <v>0.12599999</v>
+      </c>
+      <c r="J21">
+        <v>0.8999998</v>
+      </c>
+      <c r="K21">
+        <v>0.068000006</v>
+      </c>
+      <c r="L21">
+        <v>1.2950001</v>
+      </c>
+      <c r="M21">
+        <v>0.60699998</v>
+      </c>
+      <c r="N21">
+        <v>2.679098546</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <v>2011</v>
+      </c>
+      <c r="B22">
+        <v>32.316314</v>
+      </c>
+      <c r="C22">
+        <v>1.3819999</v>
+      </c>
+      <c r="D22">
+        <v>1.9595741</v>
+      </c>
+      <c r="E22">
+        <v>7.91</v>
+      </c>
+      <c r="F22">
+        <v>0.50045303</v>
+      </c>
+      <c r="G22">
+        <v>9.5389998</v>
+      </c>
+      <c r="H22">
+        <v>1.2959997</v>
+      </c>
+      <c r="I22">
+        <v>0.08020001</v>
+      </c>
+      <c r="J22">
+        <v>0.827</v>
+      </c>
+      <c r="K22">
+        <v>0.904999994</v>
+      </c>
+      <c r="L22">
+        <v>2.2615001</v>
+      </c>
+      <c r="M22">
+        <v>2.0860002</v>
+      </c>
+      <c r="N22">
+        <v>3.569587166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <v>2012</v>
+      </c>
+      <c r="B23">
+        <v>30.302495</v>
+      </c>
+      <c r="C23">
+        <v>1.3260003</v>
+      </c>
+      <c r="D23">
+        <v>1.3551799</v>
+      </c>
+      <c r="E23">
+        <v>8.161003</v>
+      </c>
+      <c r="F23">
+        <v>0.41626697</v>
+      </c>
+      <c r="G23">
+        <v>3.654002</v>
+      </c>
+      <c r="H23">
+        <v>1.7180004</v>
+      </c>
+      <c r="I23">
+        <v>0.29399995</v>
+      </c>
+      <c r="J23">
+        <v>1.1370002</v>
+      </c>
+      <c r="K23">
+        <v>0.7540001</v>
+      </c>
+      <c r="L23">
+        <v>2.9695007</v>
+      </c>
+      <c r="M23">
+        <v>3.6109998</v>
+      </c>
+      <c r="N23">
+        <v>4.90654168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <v>2013</v>
+      </c>
+      <c r="B24">
+        <v>36.302525</v>
+      </c>
+      <c r="C24">
+        <v>0.769</v>
+      </c>
+      <c r="D24">
+        <v>0.9185354</v>
+      </c>
+      <c r="E24">
+        <v>2.633</v>
+      </c>
+      <c r="F24">
+        <v>0.6172451</v>
+      </c>
+      <c r="G24">
+        <v>1.400349</v>
+      </c>
+      <c r="H24">
+        <v>6.9670006</v>
+      </c>
+      <c r="I24">
+        <v>0.531</v>
+      </c>
+      <c r="J24">
+        <v>0.4250632</v>
+      </c>
+      <c r="K24">
+        <v>1.1829999</v>
+      </c>
+      <c r="L24">
+        <v>3.712879</v>
+      </c>
+      <c r="M24">
+        <v>11.040002</v>
+      </c>
+      <c r="N24">
+        <v>6.1054508</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <v>2014</v>
+      </c>
+      <c r="B25">
+        <v>40.19752</v>
+      </c>
+      <c r="C25">
+        <v>0.7189997</v>
+      </c>
+      <c r="D25">
+        <v>0.7571286</v>
+      </c>
+      <c r="E25">
+        <v>1.189997</v>
+      </c>
+      <c r="F25">
+        <v>2.173181</v>
+      </c>
+      <c r="G25">
+        <v>0.409998999999999</v>
+      </c>
+      <c r="H25">
+        <v>9.739999</v>
+      </c>
+      <c r="I25">
+        <v>0.926</v>
+      </c>
+      <c r="J25">
+        <v>0.00699990000000028</v>
+      </c>
+      <c r="K25">
+        <v>2.5910004</v>
+      </c>
+      <c r="L25">
+        <v>5.78625</v>
+      </c>
+      <c r="M25">
+        <v>10.64</v>
+      </c>
+      <c r="N25">
+        <v>5.2579654</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <v>2015</v>
+      </c>
+      <c r="B26">
+        <v>48.20749</v>
+      </c>
+      <c r="C26">
+        <v>0.659</v>
+      </c>
+      <c r="D26">
+        <v>1.1030995</v>
+      </c>
+      <c r="E26">
+        <v>1.324003</v>
+      </c>
+      <c r="F26">
+        <v>1.9209762</v>
+      </c>
+      <c r="G26">
+        <v>0.307002000000001</v>
+      </c>
+      <c r="H26">
+        <v>10.811</v>
+      </c>
+      <c r="I26">
+        <v>1.134</v>
+      </c>
+      <c r="J26">
+        <v>0.00699999999999967</v>
+      </c>
+      <c r="K26">
+        <v>4.0732196</v>
+      </c>
+      <c r="L26">
+        <v>6.124717</v>
+      </c>
+      <c r="M26">
+        <v>15.149998</v>
+      </c>
+      <c r="N26">
+        <v>5.59347469999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27">
+        <v>2016</v>
+      </c>
+      <c r="B27">
+        <v>72.16273</v>
+      </c>
+      <c r="C27">
+        <v>0.743</v>
+      </c>
+      <c r="D27">
+        <v>0.564563499999999</v>
+      </c>
+      <c r="E27">
+        <v>1.454997</v>
+      </c>
+      <c r="F27">
+        <v>4.2855377</v>
+      </c>
+      <c r="G27">
+        <v>0.382000000000001</v>
+      </c>
+      <c r="H27">
+        <v>7.89</v>
+      </c>
+      <c r="I27">
+        <v>0.8870006</v>
+      </c>
+      <c r="J27">
+        <v>0.00899970000000039</v>
+      </c>
+      <c r="K27">
+        <v>2.312801</v>
+      </c>
+      <c r="L27">
+        <v>11.196831</v>
+      </c>
+      <c r="M27">
+        <v>34.27</v>
+      </c>
+      <c r="N27">
+        <v>8.1669995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28">
+        <v>2017</v>
+      </c>
+      <c r="B28">
+        <v>94.86436</v>
+      </c>
+      <c r="C28">
+        <v>0.6650006</v>
+      </c>
+      <c r="D28">
+        <v>0.908355999999999</v>
+      </c>
+      <c r="E28">
+        <v>1.614003</v>
+      </c>
+      <c r="F28">
+        <v>8.272735</v>
+      </c>
+      <c r="G28">
+        <v>0.399291999999999</v>
+      </c>
+      <c r="H28">
+        <v>7.460004</v>
+      </c>
+      <c r="I28">
+        <v>1.3329997</v>
+      </c>
+      <c r="J28">
+        <v>0.0100004</v>
+      </c>
+      <c r="K28">
+        <v>0.845999000000001</v>
+      </c>
+      <c r="L28">
+        <v>8.336162</v>
+      </c>
+      <c r="M28">
+        <v>53.01349</v>
+      </c>
+      <c r="N28">
+        <v>12.0063183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29">
+        <v>2018</v>
+      </c>
+      <c r="B29">
+        <v>93.3594</v>
+      </c>
+      <c r="C29">
+        <v>1.2719994</v>
+      </c>
+      <c r="D29">
+        <v>1.06186</v>
+      </c>
+      <c r="E29">
+        <v>2.864997</v>
+      </c>
+      <c r="F29">
+        <v>9.201341</v>
+      </c>
+      <c r="G29">
+        <v>0.425294999999998</v>
+      </c>
+      <c r="H29">
+        <v>6.661999</v>
+      </c>
+      <c r="I29">
+        <v>2.2637997</v>
+      </c>
+      <c r="J29">
+        <v>0.0406068999999993</v>
+      </c>
+      <c r="K29">
+        <v>0.299050999999999</v>
+      </c>
+      <c r="L29">
+        <v>8.217156</v>
+      </c>
+      <c r="M29">
+        <v>44.42958</v>
+      </c>
+      <c r="N29">
+        <v>16.621715</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30">
+        <v>2019</v>
+      </c>
+      <c r="B30">
+        <v>102.9386</v>
+      </c>
+      <c r="C30">
+        <v>4.344</v>
+      </c>
+      <c r="D30">
+        <v>1.1445775</v>
+      </c>
+      <c r="E30">
+        <v>3.756</v>
+      </c>
+      <c r="F30">
+        <v>7.750309</v>
+      </c>
+      <c r="G30">
+        <v>0.757688000000002</v>
+      </c>
+      <c r="H30">
+        <v>7.029997</v>
+      </c>
+      <c r="I30">
+        <v>3.853001</v>
+      </c>
+      <c r="J30">
+        <v>4.0435407</v>
+      </c>
+      <c r="K30">
+        <v>0.1649595</v>
+      </c>
+      <c r="L30">
+        <v>9.600238</v>
+      </c>
+      <c r="M30">
+        <v>29.70894</v>
+      </c>
+      <c r="N30">
+        <v>30.7853493</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>2020</v>
+      </c>
+      <c r="B31">
+        <v>128.1841</v>
+      </c>
+      <c r="C31">
+        <v>5.016</v>
+      </c>
+      <c r="D31">
+        <v>1.2481005</v>
+      </c>
+      <c r="E31">
+        <v>4.757</v>
+      </c>
+      <c r="F31">
+        <v>4.181753</v>
+      </c>
+      <c r="G31">
+        <v>0.784763000000002</v>
+      </c>
+      <c r="H31">
+        <v>6.572</v>
+      </c>
+      <c r="I31">
+        <v>2.622791</v>
+      </c>
+      <c r="J31">
+        <v>1.32839</v>
+      </c>
+      <c r="K31">
+        <v>0.238451000000001</v>
+      </c>
+      <c r="L31">
+        <v>14.853866</v>
+      </c>
+      <c r="M31">
+        <v>48.99299</v>
+      </c>
+      <c r="N31">
+        <v>37.5879955</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>2021</v>
+      </c>
+      <c r="B32">
+        <v>141.1086</v>
+      </c>
+      <c r="C32">
+        <v>4.884</v>
+      </c>
+      <c r="D32">
+        <v>2.754409</v>
+      </c>
+      <c r="E32">
+        <v>5.702</v>
+      </c>
+      <c r="F32">
+        <v>10.29885</v>
+      </c>
+      <c r="G32">
+        <v>0.944216999999998</v>
+      </c>
+      <c r="H32">
+        <v>4.42700000000001</v>
+      </c>
+      <c r="I32">
+        <v>3.585784</v>
+      </c>
+      <c r="J32">
+        <v>3.579608</v>
+      </c>
+      <c r="K32">
+        <v>0.3365385</v>
+      </c>
+      <c r="L32">
+        <v>18.949815</v>
+      </c>
+      <c r="M32">
+        <v>53.00904</v>
+      </c>
+      <c r="N32">
+        <v>32.6373385</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>2022</v>
+      </c>
+      <c r="B33">
+        <v>191.5781</v>
+      </c>
+      <c r="C33">
+        <v>3.922002</v>
+      </c>
+      <c r="D33">
+        <v>2.6</v>
+      </c>
+      <c r="E33">
+        <v>7.181</v>
+      </c>
+      <c r="F33">
+        <v>13.462074</v>
+      </c>
+      <c r="G33">
+        <v>2.482301</v>
+      </c>
+      <c r="H33">
+        <v>4.642</v>
+      </c>
+      <c r="I33">
+        <v>2.814146</v>
+      </c>
+      <c r="J33">
+        <v>4.498331</v>
+      </c>
+      <c r="K33">
+        <v>0.612900999999999</v>
+      </c>
+      <c r="L33">
+        <v>17.624135</v>
+      </c>
+      <c r="M33">
+        <v>86.05899</v>
+      </c>
+      <c r="N33">
+        <v>45.68022</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>2023</v>
+      </c>
+      <c r="B34">
+        <v>345.833451</v>
+      </c>
+      <c r="C34">
+        <v>3.725</v>
+      </c>
+      <c r="D34">
+        <v>3.201</v>
+      </c>
+      <c r="E34">
+        <v>14.26</v>
+      </c>
+      <c r="F34">
+        <v>9.48853</v>
+      </c>
+      <c r="G34">
+        <v>5.234</v>
+      </c>
+      <c r="H34">
+        <v>4.011</v>
+      </c>
+      <c r="I34">
+        <v>2.968086</v>
+      </c>
+      <c r="J34">
+        <v>5.401</v>
+      </c>
+      <c r="K34">
+        <v>1.0055</v>
+      </c>
+      <c r="L34">
+        <v>24.84433</v>
+      </c>
+      <c r="M34">
+        <v>216.88</v>
+      </c>
+      <c r="N34">
+        <v>54.815005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:P36"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="10.375"/>
+    <col min="3" max="4" width="11.5"/>
+    <col min="5" max="5" width="10.375"/>
+    <col min="6" max="7" width="11.5"/>
+    <col min="8" max="8" width="10.375"/>
+    <col min="9" max="9" width="9.375"/>
+    <col min="10" max="12" width="10.375"/>
+    <col min="13" max="14" width="11.5"/>
+    <col min="15" max="15" width="10.375"/>
+    <col min="16" max="16" width="12.625"/>
+    <col min="17" max="17" width="11.5"/>
+    <col min="18" max="19" width="10.375"/>
+    <col min="20" max="20" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>2179.354</v>
+      </c>
+      <c r="C2">
+        <v>2665.29</v>
+      </c>
+      <c r="D2">
+        <v>2684.72</v>
+      </c>
+      <c r="E2">
+        <v>2548.02</v>
+      </c>
+      <c r="F2">
+        <v>2612.51</v>
+      </c>
+      <c r="G2">
+        <v>2866.2</v>
+      </c>
+      <c r="H2">
+        <v>2493.25</v>
+      </c>
+      <c r="I2">
+        <v>1537.46</v>
+      </c>
+      <c r="J2">
+        <v>2748.21</v>
+      </c>
+      <c r="K2">
+        <v>3021.82</v>
+      </c>
+      <c r="L2">
+        <v>2779.05</v>
+      </c>
+      <c r="M2">
+        <v>2711.49</v>
+      </c>
+      <c r="N2">
+        <v>2926.17</v>
+      </c>
+      <c r="O2">
+        <v>1662.85</v>
+      </c>
+      <c r="P2">
+        <v>2358.98928379879</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>2143.23</v>
+      </c>
+      <c r="C3">
+        <v>2866.67</v>
+      </c>
+      <c r="D3">
+        <v>2658.63</v>
+      </c>
+      <c r="E3">
+        <v>2548.02</v>
+      </c>
+      <c r="F3">
+        <v>2403.5</v>
+      </c>
+      <c r="G3">
+        <v>3516.01</v>
+      </c>
+      <c r="H3">
+        <v>2647.02</v>
+      </c>
+      <c r="I3">
+        <v>1362.27</v>
+      </c>
+      <c r="J3">
+        <v>2673.59</v>
+      </c>
+      <c r="K3">
+        <v>2787.11</v>
+      </c>
+      <c r="L3">
+        <v>2491.62</v>
+      </c>
+      <c r="M3">
+        <v>2510.34</v>
+      </c>
+      <c r="N3">
+        <v>2897.74</v>
+      </c>
+      <c r="O3">
+        <v>1617.71</v>
+      </c>
+      <c r="P3">
+        <v>2760.56497665597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>2039.148</v>
+      </c>
+      <c r="C4">
+        <v>2309.92</v>
+      </c>
+      <c r="D4">
+        <v>2433.3</v>
+      </c>
+      <c r="E4">
+        <v>2314.87</v>
+      </c>
+      <c r="F4">
+        <v>2614.37</v>
+      </c>
+      <c r="G4">
+        <v>3289.66</v>
+      </c>
+      <c r="H4">
+        <v>2588.59</v>
+      </c>
+      <c r="I4">
+        <v>1627.21</v>
+      </c>
+      <c r="J4">
+        <v>2345.46</v>
+      </c>
+      <c r="K4">
+        <v>3036.31</v>
+      </c>
+      <c r="L4">
+        <v>2260.92</v>
+      </c>
+      <c r="M4">
+        <v>1987</v>
+      </c>
+      <c r="N4">
+        <v>2942.56</v>
+      </c>
+      <c r="O4">
+        <v>1582.55</v>
+      </c>
+      <c r="P4">
+        <v>1402.27055172102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>2098.63</v>
+      </c>
+      <c r="C5">
+        <v>2514.85</v>
+      </c>
+      <c r="D5">
+        <v>2251.46</v>
+      </c>
+      <c r="E5">
+        <v>2286.82</v>
+      </c>
+      <c r="F5">
+        <v>2253.33</v>
+      </c>
+      <c r="G5">
+        <v>2269.51</v>
+      </c>
+      <c r="H5">
+        <v>2601.18</v>
+      </c>
+      <c r="I5">
+        <v>1672.43</v>
+      </c>
+      <c r="J5">
+        <v>2334.8</v>
+      </c>
+      <c r="K5">
+        <v>2930.69</v>
+      </c>
+      <c r="L5">
+        <v>2130.88</v>
+      </c>
+      <c r="M5">
+        <v>2191.18</v>
+      </c>
+      <c r="N5">
+        <v>2934.81</v>
+      </c>
+      <c r="O5">
+        <v>1503.32</v>
+      </c>
+      <c r="P5">
+        <v>3011.18340125676</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>2029.72</v>
+      </c>
+      <c r="C6">
+        <v>2323.545</v>
+      </c>
+      <c r="D6">
+        <v>2136.02</v>
+      </c>
+      <c r="E6">
+        <v>2256.06</v>
+      </c>
+      <c r="F6">
+        <v>2407.15</v>
+      </c>
+      <c r="G6">
+        <v>2224.63</v>
+      </c>
+      <c r="H6">
+        <v>2541.23</v>
+      </c>
+      <c r="I6">
+        <v>1592.44</v>
+      </c>
+      <c r="J6">
+        <v>1966.64</v>
+      </c>
+      <c r="K6">
+        <v>2741.04</v>
+      </c>
+      <c r="L6">
+        <v>2013.38</v>
+      </c>
+      <c r="M6">
+        <v>2115.98</v>
+      </c>
+      <c r="N6">
+        <v>2492.83</v>
+      </c>
+      <c r="O6">
+        <v>1526.31</v>
+      </c>
+      <c r="P6">
+        <v>3013.46123961328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>1842.958</v>
+      </c>
+      <c r="C7">
+        <v>2132.24</v>
+      </c>
+      <c r="D7">
+        <v>2042.92</v>
+      </c>
+      <c r="E7">
+        <v>2214.04</v>
+      </c>
+      <c r="F7">
+        <v>2152.44</v>
+      </c>
+      <c r="G7">
+        <v>2381.01</v>
+      </c>
+      <c r="H7">
+        <v>2503.18</v>
+      </c>
+      <c r="I7">
+        <v>1429.27</v>
+      </c>
+      <c r="J7">
+        <v>1859.57</v>
+      </c>
+      <c r="K7">
+        <v>2831.48</v>
+      </c>
+      <c r="L7">
+        <v>2008.11</v>
+      </c>
+      <c r="M7">
+        <v>2179.48</v>
+      </c>
+      <c r="N7">
+        <v>2162.94</v>
+      </c>
+      <c r="O7">
+        <v>1481.82</v>
+      </c>
+      <c r="P7">
+        <v>2625.09044991796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>1847.535</v>
+      </c>
+      <c r="C8">
+        <v>2132.24</v>
+      </c>
+      <c r="D8">
+        <v>2088.4</v>
+      </c>
+      <c r="E8">
+        <v>2171.83</v>
+      </c>
+      <c r="F8">
+        <v>1979.8</v>
+      </c>
+      <c r="G8">
+        <v>2006.4</v>
+      </c>
+      <c r="H8">
+        <v>2346.94</v>
+      </c>
+      <c r="I8">
+        <v>1314.74</v>
+      </c>
+      <c r="J8">
+        <v>1831.92</v>
+      </c>
+      <c r="K8">
+        <v>2651.93</v>
+      </c>
+      <c r="L8">
+        <v>1986.94</v>
+      </c>
+      <c r="M8">
+        <v>2197.47</v>
+      </c>
+      <c r="N8">
+        <v>2267.32</v>
+      </c>
+      <c r="O8">
+        <v>1476.56</v>
+      </c>
+      <c r="P8">
+        <v>2035.27530016356</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>1849.301</v>
+      </c>
+      <c r="C9">
+        <v>1964.61</v>
+      </c>
+      <c r="D9">
+        <v>1890.91</v>
+      </c>
+      <c r="E9">
+        <v>2171.49</v>
+      </c>
+      <c r="F9">
+        <v>1794.22</v>
+      </c>
+      <c r="G9">
+        <v>2870.95</v>
+      </c>
+      <c r="H9">
+        <v>2370.73</v>
+      </c>
+      <c r="I9">
+        <v>1299.89</v>
+      </c>
+      <c r="J9">
+        <v>2010.69</v>
+      </c>
+      <c r="K9">
+        <v>2328.18</v>
+      </c>
+      <c r="L9">
+        <v>2263.38</v>
+      </c>
+      <c r="M9">
+        <v>1983.35</v>
+      </c>
+      <c r="N9">
+        <v>1946.23</v>
+      </c>
+      <c r="O9">
+        <v>1399.04</v>
+      </c>
+      <c r="P9">
+        <v>2539.29275064451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>1754.856</v>
+      </c>
+      <c r="C10">
+        <v>2134.65</v>
+      </c>
+      <c r="D10">
+        <v>1843.69</v>
+      </c>
+      <c r="E10">
+        <v>2135.76</v>
+      </c>
+      <c r="F10">
+        <v>1431.96</v>
+      </c>
+      <c r="G10">
+        <v>1972.42</v>
+      </c>
+      <c r="H10">
+        <v>2070.96</v>
+      </c>
+      <c r="I10">
+        <v>1301.17</v>
+      </c>
+      <c r="J10">
+        <v>2624.35</v>
+      </c>
+      <c r="K10">
+        <v>2082.56</v>
+      </c>
+      <c r="L10">
+        <v>2186.03</v>
+      </c>
+      <c r="M10">
+        <v>2103.29</v>
+      </c>
+      <c r="N10">
+        <v>1975.47</v>
+      </c>
+      <c r="O10">
+        <v>1449.6</v>
+      </c>
+      <c r="P10">
+        <v>2113.76941159381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>1662.38</v>
+      </c>
+      <c r="C11">
+        <v>2131.67</v>
+      </c>
+      <c r="D11">
+        <v>1742.54</v>
+      </c>
+      <c r="E11">
+        <v>1976.94</v>
+      </c>
+      <c r="F11">
+        <v>1502.86</v>
+      </c>
+      <c r="G11">
+        <v>1873.63</v>
+      </c>
+      <c r="H11">
+        <v>2127.66</v>
+      </c>
+      <c r="I11">
+        <v>1182.93</v>
+      </c>
+      <c r="J11">
+        <v>1740.92</v>
+      </c>
+      <c r="K11">
+        <v>2726.55</v>
+      </c>
+      <c r="L11">
+        <v>1979.96</v>
+      </c>
+      <c r="M11">
+        <v>1887.82</v>
+      </c>
+      <c r="N11">
+        <v>1748.02</v>
+      </c>
+      <c r="O11">
+        <v>1371.4</v>
+      </c>
+      <c r="P11">
+        <v>2201.55451907036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>1496.348</v>
+      </c>
+      <c r="C12">
+        <v>2131.67</v>
+      </c>
+      <c r="D12">
+        <v>1540.47</v>
+      </c>
+      <c r="E12">
+        <v>1968.01</v>
+      </c>
+      <c r="F12">
+        <v>1505.72</v>
+      </c>
+      <c r="G12">
+        <v>1919.21</v>
+      </c>
+      <c r="H12">
+        <v>1928.72</v>
+      </c>
+      <c r="I12">
+        <v>1151.2</v>
+      </c>
+      <c r="J12">
+        <v>1366.15</v>
+      </c>
+      <c r="K12">
+        <v>1562.5</v>
+      </c>
+      <c r="L12">
+        <v>1718.01</v>
+      </c>
+      <c r="M12">
+        <v>1493.55</v>
+      </c>
+      <c r="N12">
+        <v>1606.06</v>
+      </c>
+      <c r="O12">
+        <v>1401.47</v>
+      </c>
+      <c r="P12">
+        <v>1888.64554865121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>1418.182</v>
+      </c>
+      <c r="C13">
+        <v>2131.67</v>
+      </c>
+      <c r="D13">
+        <v>1478.51</v>
+      </c>
+      <c r="E13">
+        <v>1831.53</v>
+      </c>
+      <c r="F13">
+        <v>1412.77</v>
+      </c>
+      <c r="G13">
+        <v>1473.73</v>
+      </c>
+      <c r="H13">
+        <v>2075.68</v>
+      </c>
+      <c r="I13">
+        <v>990.81</v>
+      </c>
+      <c r="J13">
+        <v>1253.62</v>
+      </c>
+      <c r="K13">
+        <v>1463.89</v>
+      </c>
+      <c r="L13">
+        <v>1903.17</v>
+      </c>
+      <c r="M13">
+        <v>1370.87</v>
+      </c>
+      <c r="N13">
+        <v>1230.49</v>
+      </c>
+      <c r="O13">
+        <v>1238.57</v>
+      </c>
+      <c r="P13">
+        <v>1964.40798332495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>1274.185</v>
+      </c>
+      <c r="C14">
+        <v>2131.67</v>
+      </c>
+      <c r="D14">
+        <v>1219.41</v>
+      </c>
+      <c r="E14">
+        <v>1895.12</v>
+      </c>
+      <c r="F14">
+        <v>1237</v>
+      </c>
+      <c r="G14">
+        <v>1449.26</v>
+      </c>
+      <c r="H14">
+        <v>1482.4</v>
+      </c>
+      <c r="I14">
+        <v>1122.05</v>
+      </c>
+      <c r="J14">
+        <v>1159.11</v>
+      </c>
+      <c r="K14">
+        <v>1714.49</v>
+      </c>
+      <c r="L14">
+        <v>1917.8</v>
+      </c>
+      <c r="M14">
+        <v>1655.96</v>
+      </c>
+      <c r="N14">
+        <v>1052.45</v>
+      </c>
+      <c r="O14">
+        <v>1102.91</v>
+      </c>
+      <c r="P14">
+        <v>1596.07574731528</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>1118.044</v>
+      </c>
+      <c r="C15">
+        <v>2131.67</v>
+      </c>
+      <c r="D15">
+        <v>1446.71</v>
+      </c>
+      <c r="E15">
+        <v>1686.7</v>
+      </c>
+      <c r="F15">
+        <v>1479.48</v>
+      </c>
+      <c r="G15">
+        <v>1319.48</v>
+      </c>
+      <c r="H15">
+        <v>1226.96</v>
+      </c>
+      <c r="I15">
+        <v>1164.31</v>
+      </c>
+      <c r="J15">
+        <v>1116.12</v>
+      </c>
+      <c r="K15">
+        <v>1368.64</v>
+      </c>
+      <c r="L15">
+        <v>1682.85</v>
+      </c>
+      <c r="M15">
+        <v>1382.13</v>
+      </c>
+      <c r="N15">
+        <v>1039.97</v>
+      </c>
+      <c r="O15">
+        <v>950.34</v>
+      </c>
+      <c r="P15" cm="1">
+        <f t="array" ref="P15">(B15*B36-SUM(C15:O15*C36:O36))/P36</f>
+        <v>1499.08396690286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" t="s">
+        <v>2</v>
+      </c>
+      <c r="P22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <v>2010</v>
+      </c>
+      <c r="B23">
+        <v>30.94308</v>
+      </c>
+      <c r="C23">
+        <v>0.3197422</v>
+      </c>
+      <c r="D23">
+        <v>5.053894</v>
+      </c>
+      <c r="E23">
+        <v>1.171002</v>
+      </c>
+      <c r="F23">
+        <v>0.5420002</v>
+      </c>
+      <c r="G23">
+        <v>0.915</v>
+      </c>
+      <c r="H23">
+        <v>0.9990001</v>
+      </c>
+      <c r="I23">
+        <v>2.259001</v>
+      </c>
+      <c r="J23">
+        <v>1.517</v>
+      </c>
+      <c r="K23">
+        <v>0.6850002</v>
+      </c>
+      <c r="L23">
+        <v>1.3299997</v>
+      </c>
+      <c r="M23">
+        <v>0.52799994</v>
+      </c>
+      <c r="N23">
+        <v>0.32499999</v>
+      </c>
+      <c r="O23">
+        <v>12.03407</v>
+      </c>
+      <c r="P23">
+        <v>2.77537063999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24">
+        <v>2011</v>
+      </c>
+      <c r="B24">
+        <v>39.1586</v>
+      </c>
+      <c r="C24">
+        <v>0.1501517</v>
+      </c>
+      <c r="D24">
+        <v>6.445273</v>
+      </c>
+      <c r="E24">
+        <v>1.809</v>
+      </c>
+      <c r="F24">
+        <v>0.747</v>
+      </c>
+      <c r="G24">
+        <v>1.124</v>
+      </c>
+      <c r="H24">
+        <v>1.1749995</v>
+      </c>
+      <c r="I24">
+        <v>2.994999</v>
+      </c>
+      <c r="J24">
+        <v>0.836001</v>
+      </c>
+      <c r="K24">
+        <v>1.2980001</v>
+      </c>
+      <c r="L24">
+        <v>0.8460166</v>
+      </c>
+      <c r="M24">
+        <v>0.4090001</v>
+      </c>
+      <c r="N24">
+        <v>0.49900005</v>
+      </c>
+      <c r="O24">
+        <v>16.721123</v>
+      </c>
+      <c r="P24">
+        <v>3.67303608</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="B25">
+        <v>47.04753</v>
+      </c>
+      <c r="C25">
+        <v>0.20996</v>
+      </c>
+      <c r="D25">
+        <v>13.658334</v>
+      </c>
+      <c r="E25">
+        <v>2.267</v>
+      </c>
+      <c r="F25">
+        <v>0.842</v>
+      </c>
+      <c r="G25">
+        <v>1.184</v>
+      </c>
+      <c r="H25">
+        <v>2.434001</v>
+      </c>
+      <c r="I25">
+        <v>1.1207</v>
+      </c>
+      <c r="J25">
+        <v>1.26</v>
+      </c>
+      <c r="K25">
+        <v>0.9359997</v>
+      </c>
+      <c r="L25">
+        <v>0.8494797</v>
+      </c>
+      <c r="M25">
+        <v>0.5320001</v>
+      </c>
+      <c r="N25">
+        <v>0.4679999</v>
+      </c>
+      <c r="O25">
+        <v>15.242271</v>
+      </c>
+      <c r="P25">
+        <v>5.42778468000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="B26">
+        <v>32.738</v>
+      </c>
+      <c r="C26">
+        <v>0.656982</v>
+      </c>
+      <c r="D26">
+        <v>0.744861999999998</v>
+      </c>
+      <c r="E26">
+        <v>2.497998</v>
+      </c>
+      <c r="F26">
+        <v>0.588</v>
+      </c>
+      <c r="G26">
+        <v>0.440001000000001</v>
+      </c>
+      <c r="H26">
+        <v>2.252</v>
+      </c>
+      <c r="I26">
+        <v>1.1207</v>
+      </c>
+      <c r="J26">
+        <v>0.168998999999999</v>
+      </c>
+      <c r="K26">
+        <v>1.6000006</v>
+      </c>
+      <c r="L26">
+        <v>0.548464699999999</v>
+      </c>
+      <c r="M26">
+        <v>0.499</v>
+      </c>
+      <c r="N26">
+        <v>0.3080202</v>
+      </c>
+      <c r="O26">
+        <v>15.133666</v>
+      </c>
+      <c r="P26">
+        <v>5.32330619</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27">
+        <v>2014</v>
+      </c>
+      <c r="B27">
+        <v>49.43942</v>
+      </c>
+      <c r="C27">
+        <v>0.0674799999999998</v>
+      </c>
+      <c r="D27">
+        <v>4.232024</v>
+      </c>
+      <c r="E27">
+        <v>5.137002</v>
+      </c>
+      <c r="F27">
+        <v>0.8940001</v>
+      </c>
+      <c r="G27">
+        <v>0.141</v>
+      </c>
+      <c r="H27">
+        <v>1.791999</v>
+      </c>
+      <c r="I27">
+        <v>4.044902</v>
+      </c>
+      <c r="J27">
+        <v>-0.0329989999999967</v>
+      </c>
+      <c r="K27">
+        <v>1.8929994</v>
+      </c>
+      <c r="L27">
+        <v>1.045465</v>
+      </c>
+      <c r="M27">
+        <v>0.8699998</v>
+      </c>
+      <c r="N27">
+        <v>2.6860332</v>
+      </c>
+      <c r="O27">
+        <v>20.0886</v>
+      </c>
+      <c r="P27">
+        <v>5.86191458</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <v>2015</v>
+      </c>
+      <c r="B28">
+        <v>66.88092</v>
+      </c>
+      <c r="C28">
+        <v>0.1905633</v>
+      </c>
+      <c r="D28">
+        <v>8.337045</v>
+      </c>
+      <c r="E28">
+        <v>5.965998</v>
+      </c>
+      <c r="F28">
+        <v>0.7309999</v>
+      </c>
+      <c r="G28">
+        <v>0.453999</v>
+      </c>
+      <c r="H28">
+        <v>1.231741</v>
+      </c>
+      <c r="I28">
+        <v>2.622888</v>
+      </c>
+      <c r="J28">
+        <v>0.0179989999999997</v>
+      </c>
+      <c r="K28">
+        <v>1.520001</v>
+      </c>
+      <c r="L28">
+        <v>1.096752</v>
+      </c>
+      <c r="M28">
+        <v>0.8730003</v>
+      </c>
+      <c r="N28">
+        <v>2.7450626</v>
+      </c>
+      <c r="O28">
+        <v>34.22859</v>
+      </c>
+      <c r="P28">
+        <v>6.19228108999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29">
+        <v>2016</v>
+      </c>
+      <c r="B29">
+        <v>50.68139</v>
+      </c>
+      <c r="C29">
+        <v>0.1681762</v>
+      </c>
+      <c r="D29">
+        <v>8.73513</v>
+      </c>
+      <c r="E29">
+        <v>4.855</v>
+      </c>
+      <c r="F29">
+        <v>0.6160002</v>
+      </c>
+      <c r="G29">
+        <v>0.247000999999999</v>
+      </c>
+      <c r="H29">
+        <v>1.820189</v>
+      </c>
+      <c r="I29">
+        <v>3.612251</v>
+      </c>
+      <c r="J29">
+        <v>0.0470019999999991</v>
+      </c>
+      <c r="K29">
+        <v>0.759</v>
+      </c>
+      <c r="L29">
+        <v>1.268384</v>
+      </c>
+      <c r="M29">
+        <v>1.2480001</v>
+      </c>
+      <c r="N29">
+        <v>2.49604</v>
+      </c>
+      <c r="O29">
+        <v>17.46916</v>
+      </c>
+      <c r="P29">
+        <v>6.53805596000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <v>2017</v>
+      </c>
+      <c r="B30">
+        <v>47.39437</v>
+      </c>
+      <c r="C30">
+        <v>0.2438068</v>
+      </c>
+      <c r="D30">
+        <v>6.328425</v>
+      </c>
+      <c r="E30">
+        <v>6.145</v>
+      </c>
+      <c r="F30">
+        <v>0.1760001</v>
+      </c>
+      <c r="G30">
+        <v>0.352578000000001</v>
+      </c>
+      <c r="H30">
+        <v>3.459071</v>
+      </c>
+      <c r="I30">
+        <v>4.148019</v>
+      </c>
+      <c r="J30">
+        <v>0.134477999999998</v>
+      </c>
+      <c r="K30">
+        <v>0.276999999999999</v>
+      </c>
+      <c r="L30">
+        <v>1.93279</v>
+      </c>
+      <c r="M30">
+        <v>0.7651496</v>
+      </c>
+      <c r="N30">
+        <v>2.175117</v>
+      </c>
+      <c r="O30">
+        <v>15.85761</v>
+      </c>
+      <c r="P30">
+        <v>4.52732549999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31">
+        <v>2018</v>
+      </c>
+      <c r="B31">
+        <v>50.0899999999999</v>
+      </c>
+      <c r="C31">
+        <v>0.6337113</v>
+      </c>
+      <c r="D31">
+        <v>6.83540000000001</v>
+      </c>
+      <c r="E31">
+        <v>3.141004</v>
+      </c>
+      <c r="F31">
+        <v>0.6889995</v>
+      </c>
+      <c r="G31">
+        <v>0.493668</v>
+      </c>
+      <c r="H31">
+        <v>2.020349</v>
+      </c>
+      <c r="I31">
+        <v>2.439645</v>
+      </c>
+      <c r="J31">
+        <v>0.280576</v>
+      </c>
+      <c r="K31">
+        <v>0.566000000000001</v>
+      </c>
+      <c r="L31">
+        <v>1.400792</v>
+      </c>
+      <c r="M31">
+        <v>0.4892364</v>
+      </c>
+      <c r="N31">
+        <v>2.538822</v>
+      </c>
+      <c r="O31">
+        <v>20.29039</v>
+      </c>
+      <c r="P31">
+        <v>7.42140679999989</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32">
+        <v>2019</v>
+      </c>
+      <c r="B32">
+        <v>56.3285000000001</v>
+      </c>
+      <c r="C32">
+        <v>-0.0121172999999999</v>
+      </c>
+      <c r="D32">
+        <v>9.169366</v>
+      </c>
+      <c r="E32">
+        <v>2.021</v>
+      </c>
+      <c r="F32">
+        <v>1.381001</v>
+      </c>
+      <c r="G32">
+        <v>0.449214</v>
+      </c>
+      <c r="H32">
+        <v>2.276612</v>
+      </c>
+      <c r="I32">
+        <v>2.217075</v>
+      </c>
+      <c r="J32">
+        <v>2.18502</v>
+      </c>
+      <c r="K32">
+        <v>0.597</v>
+      </c>
+      <c r="L32">
+        <v>1.526709</v>
+      </c>
+      <c r="M32">
+        <v>0.5857696</v>
+      </c>
+      <c r="N32">
+        <v>0.595283999999999</v>
+      </c>
+      <c r="O32">
+        <v>24.91702</v>
+      </c>
+      <c r="P32">
+        <v>7.0525467000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33">
+        <v>2020</v>
+      </c>
+      <c r="B33">
+        <v>110.8141</v>
+      </c>
+      <c r="C33">
+        <v>0.156490300000001</v>
+      </c>
+      <c r="D33">
+        <v>14.827984</v>
+      </c>
+      <c r="E33">
+        <v>1.459</v>
+      </c>
+      <c r="F33">
+        <v>1.295</v>
+      </c>
+      <c r="G33">
+        <v>0.191162</v>
+      </c>
+      <c r="H33">
+        <v>0.602827999999999</v>
+      </c>
+      <c r="I33">
+        <v>1.053425</v>
+      </c>
+      <c r="J33">
+        <v>1.229115</v>
+      </c>
+      <c r="K33">
+        <v>0.21396</v>
+      </c>
+      <c r="L33">
+        <v>1.087145</v>
+      </c>
+      <c r="M33">
+        <v>1.241239</v>
+      </c>
+      <c r="N33">
+        <v>1.759945</v>
+      </c>
+      <c r="O33">
+        <v>72.53076</v>
+      </c>
+      <c r="P33">
+        <v>10.2872443</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34">
+        <v>2021</v>
+      </c>
+      <c r="B34">
+        <v>92.5154</v>
+      </c>
+      <c r="C34">
+        <v>0.753806399999999</v>
+      </c>
+      <c r="D34">
+        <v>14.35575</v>
+      </c>
+      <c r="E34">
+        <v>1.63200000000001</v>
+      </c>
+      <c r="F34">
+        <v>2.139999</v>
+      </c>
+      <c r="G34">
+        <v>0.383111</v>
+      </c>
+      <c r="H34">
+        <v>1.245353</v>
+      </c>
+      <c r="I34">
+        <v>1.508665</v>
+      </c>
+      <c r="J34">
+        <v>1.088461</v>
+      </c>
+      <c r="K34">
+        <v>0.676599</v>
+      </c>
+      <c r="L34">
+        <v>1.225981</v>
+      </c>
+      <c r="M34">
+        <v>1.774601</v>
+      </c>
+      <c r="N34">
+        <v>3.962946</v>
+      </c>
+      <c r="O34">
+        <v>46.86078</v>
+      </c>
+      <c r="P34">
+        <v>14.3875075</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35">
+        <v>2022</v>
+      </c>
+      <c r="B35">
+        <v>74.6534</v>
+      </c>
+      <c r="C35">
+        <v>0.0670000000000002</v>
+      </c>
+      <c r="D35">
+        <v>7.84232999999998</v>
+      </c>
+      <c r="E35">
+        <v>2.481996</v>
+      </c>
+      <c r="F35">
+        <v>2.441001</v>
+      </c>
+      <c r="G35">
+        <v>0.526</v>
+      </c>
+      <c r="H35">
+        <v>2.807199</v>
+      </c>
+      <c r="I35">
+        <v>1.862513</v>
+      </c>
+      <c r="J35">
+        <v>1.400185</v>
+      </c>
+      <c r="K35">
+        <v>0.991901</v>
+      </c>
+      <c r="L35">
+        <v>2.380001</v>
+      </c>
+      <c r="M35">
+        <v>0.789199</v>
+      </c>
+      <c r="N35">
+        <v>3.00186</v>
+      </c>
+      <c r="O35">
+        <v>36.99075</v>
+      </c>
+      <c r="P35">
+        <v>9.59360500000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36">
+        <v>2023</v>
+      </c>
+      <c r="B36">
+        <v>115.96801</v>
+      </c>
+      <c r="C36">
+        <v>0.054</v>
+      </c>
+      <c r="D36">
+        <v>6.34594899999999</v>
+      </c>
+      <c r="E36">
+        <v>3.038</v>
+      </c>
+      <c r="F36">
+        <v>1.973</v>
+      </c>
+      <c r="G36">
+        <v>0.487</v>
+      </c>
+      <c r="H36">
+        <v>0.635</v>
+      </c>
+      <c r="I36">
+        <v>2.80646</v>
+      </c>
+      <c r="J36">
+        <v>0.912</v>
+      </c>
+      <c r="K36">
+        <v>1.72444</v>
+      </c>
+      <c r="L36">
+        <v>1.385</v>
+      </c>
+      <c r="M36">
+        <v>0.301</v>
+      </c>
+      <c r="N36">
+        <v>4.971984</v>
+      </c>
+      <c r="O36">
+        <v>69.07</v>
+      </c>
+      <c r="P36">
+        <v>20.474817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>